<commit_message>
add dynamically expanding table for items so that the template doesnt get broken when we have a long list of items
</commit_message>
<xml_diff>
--- a/delivery_report_template.xlsx
+++ b/delivery_report_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nik40\Git\solar-cargo-be\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBBD3C3-21D6-412E-8557-A7A8F4EDF738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2953CBE1-4AB6-42A9-AECD-B9B01A835ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="1965" windowWidth="20505" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1965" yWindow="2160" windowWidth="20505" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -668,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -709,39 +709,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -797,7 +781,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -811,31 +797,43 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,104 +1052,105 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M991"/>
+  <dimension ref="A1:M988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="6" width="12.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="10" max="12" width="12.5703125" customWidth="1"/>
+    <col min="9" max="11" width="7.140625" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="77"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="65"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="81" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="45"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="75"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="48"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="62"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="69"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
       <c r="K4" s="3"/>
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="69"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="55"/>
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="3"/>
       <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="72"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="58"/>
       <c r="I6" s="5"/>
       <c r="J6" s="6"/>
       <c r="K6" s="7"/>
@@ -1172,210 +1171,213 @@
       <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="42"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="79"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="91"/>
-      <c r="G9" s="91"/>
-      <c r="H9" s="92"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="87"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="90"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="34"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="90"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="34"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="94"/>
-      <c r="F11" s="91"/>
-      <c r="G11" s="91"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="89"/>
-      <c r="L11" s="89"/>
-      <c r="M11" s="90"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="34"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="91"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="89"/>
-      <c r="M12" s="90"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="34"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="90"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="34"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="90"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="34"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="90"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="89"/>
-      <c r="L16" s="89"/>
-      <c r="M16" s="90"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="40" t="s">
+      <c r="B15" s="71"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="34"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="48"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="62"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="83" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="A18" s="14">
+        <v>1</v>
+      </c>
+      <c r="B18" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
-        <v>1</v>
-      </c>
-      <c r="B19" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="33"/>
+        <v>2</v>
+      </c>
+      <c r="B19" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="71"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
@@ -1383,17 +1385,17 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
-        <v>2</v>
-      </c>
-      <c r="B20" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="33"/>
+        <v>3</v>
+      </c>
+      <c r="B20" s="84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="71"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -1401,17 +1403,17 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
-        <v>3</v>
-      </c>
-      <c r="B21" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="33"/>
+        <v>4</v>
+      </c>
+      <c r="B21" s="85" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="71"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -1419,35 +1421,35 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
-        <v>4</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="15"/>
+        <v>5</v>
+      </c>
+      <c r="B22" s="85" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="17"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="16"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
-        <v>5</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="33"/>
+        <v>6</v>
+      </c>
+      <c r="B23" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="71"/>
       <c r="I23" s="17"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
@@ -1455,127 +1457,123 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
-        <v>6</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="33"/>
+        <v>7</v>
+      </c>
+      <c r="B24" s="85" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
       <c r="I24" s="17"/>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="16"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
-        <v>7</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="33"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="17"/>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
       <c r="L25" s="16"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="16"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="40" t="s">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="42"/>
+      <c r="B26" s="78"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="79"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="89"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="75"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="45"/>
+      <c r="A28" s="86" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="78"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="78"/>
+      <c r="J28" s="78"/>
+      <c r="K28" s="78"/>
+      <c r="L28" s="79"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="48"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="24"/>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="48"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="24"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="42"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="24"/>
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
@@ -1718,164 +1716,125 @@
       <c r="L41" s="24"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="24"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="26"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="24"/>
+      <c r="A43" s="90"/>
+      <c r="B43" s="91"/>
+      <c r="C43" s="91"/>
+      <c r="D43" s="91"/>
+      <c r="E43" s="91"/>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="91"/>
+      <c r="K43" s="91"/>
+      <c r="L43" s="92"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="24"/>
+      <c r="A44" s="86" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="78"/>
+      <c r="C44" s="78"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="78"/>
+      <c r="F44" s="78"/>
+      <c r="G44" s="78"/>
+      <c r="H44" s="78"/>
+      <c r="I44" s="78"/>
+      <c r="J44" s="78"/>
+      <c r="K44" s="78"/>
+      <c r="L44" s="79"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="26"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="28"/>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="50"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
-      <c r="I46" s="51"/>
-      <c r="J46" s="51"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="52"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="88"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="24"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="41"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="41"/>
-      <c r="L47" s="42"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="87" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="88"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="24"/>
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="28"/>
-    </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="38"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="24"/>
-    </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C50" s="38"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="24"/>
-    </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="29"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="31"/>
-    </row>
-    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
+      <c r="L48" s="31"/>
+    </row>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2800,34 +2759,30 @@
     <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="A3:D6"/>
-    <mergeCell ref="E3:H6"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+  <mergeCells count="54">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="A16:L16"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A8:L8"/>
@@ -2838,33 +2793,28 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="A47:L47"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A46:L46"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A3:D6"/>
+    <mergeCell ref="E3:H6"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
add get username functionality
</commit_message>
<xml_diff>
--- a/delivery_report_template.xlsx
+++ b/delivery_report_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nik40\Git\solar-cargo-be\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2953CBE1-4AB6-42A9-AECD-B9B01A835ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58512D02-AD29-4179-8A53-34F7EA1D223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="2160" windowWidth="20505" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8310" yWindow="2370" windowWidth="20505" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -668,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -714,16 +714,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -783,7 +808,6 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -793,47 +817,29 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,8 +1060,8 @@
   </sheetPr>
   <dimension ref="A1:M988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47:H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1067,90 +1073,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="65"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="83"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="69" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="75"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="49"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="62"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="57"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="55"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="74"/>
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
       <c r="K4" s="3"/>
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="55"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="74"/>
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="3"/>
       <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="58"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="77"/>
       <c r="I6" s="5"/>
       <c r="J6" s="6"/>
       <c r="K6" s="7"/>
@@ -1171,169 +1177,169 @@
       <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="79"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="46"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="71"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="35"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="92"/>
       <c r="I9" s="33"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="82"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
       <c r="M9" s="34"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="71"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="92"/>
       <c r="I10" s="32"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
       <c r="M10" s="34"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="71"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="71"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="36"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="38"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="90"/>
       <c r="M11" s="34"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="71"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="92"/>
       <c r="I12" s="32"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
       <c r="M12" s="34"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="76" t="s">
+      <c r="A13" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="71"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="38"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="92"/>
       <c r="I13" s="32"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="71"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="71"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="38"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="92"/>
       <c r="I14" s="32"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="90"/>
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="76" t="s">
+      <c r="A15" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="71"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="71"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="38"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="92"/>
       <c r="I15" s="32"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="90"/>
+      <c r="L15" s="90"/>
       <c r="M15" s="34"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="62"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="57"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="83" t="s">
+      <c r="B17" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="71"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="38"/>
       <c r="I17" s="12" t="s">
         <v>14</v>
       </c>
@@ -1351,15 +1357,15 @@
       <c r="A18" s="14">
         <v>1</v>
       </c>
-      <c r="B18" s="84" t="s">
+      <c r="B18" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="71"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="38"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -1369,15 +1375,15 @@
       <c r="A19" s="14">
         <v>2</v>
       </c>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="71"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="38"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
@@ -1387,15 +1393,15 @@
       <c r="A20" s="14">
         <v>3</v>
       </c>
-      <c r="B20" s="84" t="s">
+      <c r="B20" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="71"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="38"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -1405,15 +1411,15 @@
       <c r="A21" s="14">
         <v>4</v>
       </c>
-      <c r="B21" s="85" t="s">
+      <c r="B21" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="71"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="38"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -1423,15 +1429,15 @@
       <c r="A22" s="14">
         <v>5</v>
       </c>
-      <c r="B22" s="85" t="s">
+      <c r="B22" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="71"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="38"/>
       <c r="I22" s="17"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
@@ -1441,15 +1447,15 @@
       <c r="A23" s="14">
         <v>6</v>
       </c>
-      <c r="B23" s="85" t="s">
+      <c r="B23" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="71"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="38"/>
       <c r="I23" s="17"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
@@ -1459,15 +1465,15 @@
       <c r="A24" s="14">
         <v>7</v>
       </c>
-      <c r="B24" s="85" t="s">
+      <c r="B24" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="71"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="38"/>
       <c r="I24" s="17"/>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
@@ -1488,50 +1494,50 @@
       <c r="L25" s="16"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="78"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-      <c r="J26" s="78"/>
-      <c r="K26" s="78"/>
-      <c r="L26" s="79"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="46"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="89"/>
-      <c r="B27" s="73"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="73"/>
-      <c r="J27" s="73"/>
-      <c r="K27" s="73"/>
-      <c r="L27" s="75"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="49"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="86" t="s">
+      <c r="A28" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="78"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78"/>
-      <c r="J28" s="78"/>
-      <c r="K28" s="78"/>
-      <c r="L28" s="79"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="46"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
@@ -1730,34 +1736,34 @@
       <c r="L42" s="26"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="90"/>
-      <c r="B43" s="91"/>
-      <c r="C43" s="91"/>
-      <c r="D43" s="91"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="91"/>
-      <c r="H43" s="91"/>
-      <c r="I43" s="91"/>
-      <c r="J43" s="91"/>
-      <c r="K43" s="91"/>
-      <c r="L43" s="92"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="53"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="86" t="s">
+      <c r="A44" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="78"/>
-      <c r="C44" s="78"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="78"/>
-      <c r="J44" s="78"/>
-      <c r="K44" s="78"/>
-      <c r="L44" s="79"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="45"/>
+      <c r="L44" s="46"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
@@ -1775,15 +1781,15 @@
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
-      <c r="B46" s="87" t="s">
+      <c r="B46" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C46" s="88"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="93"/>
+      <c r="E46" s="93"/>
+      <c r="F46" s="93"/>
+      <c r="G46" s="93"/>
+      <c r="H46" s="93"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -1791,15 +1797,15 @@
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="23"/>
-      <c r="B47" s="87" t="s">
+      <c r="B47" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="88"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="94"/>
+      <c r="E47" s="94"/>
+      <c r="F47" s="94"/>
+      <c r="G47" s="94"/>
+      <c r="H47" s="94"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
@@ -2760,28 +2766,24 @@
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="54">
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="A43:L43"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
+  <mergeCells count="56">
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A3:D6"/>
+    <mergeCell ref="E3:H6"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="A16:L16"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
@@ -2793,28 +2795,34 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A3:D6"/>
-    <mergeCell ref="E3:H6"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="D46:H46"/>
+    <mergeCell ref="D47:H47"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
improvements in report generation
</commit_message>
<xml_diff>
--- a/delivery_report_template.xlsx
+++ b/delivery_report_template.xlsx
@@ -339,13 +339,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="medium"/>
       <top style="thin"/>
@@ -383,6 +376,13 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
@@ -543,15 +543,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -567,11 +567,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -579,11 +579,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -591,7 +591,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -603,7 +603,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -619,7 +619,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -627,7 +627,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -651,7 +651,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -920,7 +920,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O47" activeCellId="0" sqref="O47"/>
+      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
improved Excel + pdf template and move additional images to new sheets
</commit_message>
<xml_diff>
--- a/delivery_report_template.xlsx
+++ b/delivery_report_template.xlsx
@@ -116,14 +116,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -165,12 +164,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -246,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -270,37 +263,9 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right/>
+      <right style="thin"/>
       <top style="thin"/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -381,8 +346,43 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
@@ -434,7 +434,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -459,39 +459,115 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -499,171 +575,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -737,6 +697,49 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>192600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>172440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>801000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image3.png" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7783920" y="572400"/>
+          <a:ext cx="1618200" cy="408600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -920,7 +923,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
+      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -959,713 +962,714 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="8"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="17"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="17"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="20"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="20"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="28"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="28"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="28"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="28"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="28"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="28"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="28"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="32" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="32" t="s">
+      <c r="J17" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="32" t="s">
+      <c r="K17" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="33" t="s">
+      <c r="L17" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34" t="n">
+      <c r="A18" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="37"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="24"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34" t="n">
+      <c r="A19" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="37"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="24"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34" t="n">
+      <c r="A20" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="37"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="24"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34" t="n">
+      <c r="A21" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="37"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="24"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="34" t="n">
+      <c r="A22" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="37"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="24"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34" t="n">
+      <c r="A23" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="37"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="24"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="34" t="n">
+      <c r="A24" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="37"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="24"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="40"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="37"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="46"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="47"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="35"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="46"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="47"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="35"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="46"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="47"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="35"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="46"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="47"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="35"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="46"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="47"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="35"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="46"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="47"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="35"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="46"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="47"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="34"/>
+      <c r="L35" s="35"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="46"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="47"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="35"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="46"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="47"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
+      <c r="K37" s="34"/>
+      <c r="L37" s="35"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="46"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="47"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
+      <c r="K38" s="34"/>
+      <c r="L38" s="35"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="46"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="47"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="35"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="46"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="47"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="35"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="46"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="47"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="34"/>
+      <c r="L41" s="35"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="48"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="49"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="38"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="45" t="s">
+      <c r="A43" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="45"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="50"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="51"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="41"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="46"/>
-      <c r="B45" s="52" t="s">
+      <c r="A45" s="33"/>
+      <c r="B45" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="52"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="47"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="35"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="46"/>
-      <c r="B46" s="52" t="s">
+      <c r="A46" s="33"/>
+      <c r="B46" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="52"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="54"/>
-      <c r="G46" s="54"/>
-      <c r="H46" s="54"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="47"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="35"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="55"/>
-      <c r="B47" s="56"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="56"/>
-      <c r="L47" s="57"/>
+      <c r="A47" s="45"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="47"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2609,10 +2613,11 @@
     <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="52">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:L7"/>
     <mergeCell ref="A3:D7"/>
     <mergeCell ref="E3:H7"/>
     <mergeCell ref="A8:L8"/>
@@ -2664,10 +2669,11 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved PDF report generation
</commit_message>
<xml_diff>
--- a/delivery_report_template.xlsx
+++ b/delivery_report_template.xlsx
@@ -64,10 +64,10 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nok</t>
+    <t xml:space="preserve">Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not ok</t>
   </si>
   <si>
     <t xml:space="preserve">N/A</t>
@@ -239,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -263,7 +263,7 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="thin"/>
+      <right style="medium"/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
@@ -332,13 +332,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right/>
       <top/>
@@ -382,9 +375,9 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="medium"/>
+      <right/>
       <top style="thin"/>
-      <bottom/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -434,7 +427,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -520,11 +513,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -532,33 +525,17 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -567,11 +544,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -579,10 +564,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -595,35 +576,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -710,9 +683,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>801000</xdr:colOff>
+      <xdr:colOff>800280</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -726,7 +699,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7783920" y="572400"/>
-          <a:ext cx="1618200" cy="408600"/>
+          <a:ext cx="1617480" cy="407880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -918,12 +891,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr fitToPage="true"/>
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P30" activeCellId="0" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1340,337 +1313,324 @@
       <c r="L24" s="24"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="24"/>
+      <c r="A25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
+      <c r="A27" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="31"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="33"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="35"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="31"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="33"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="35"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="31"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="33"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="35"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="31"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="33"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="35"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="31"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="33"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="35"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="31"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="33"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="35"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="31"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="33"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="35"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="31"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="33"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="35"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="31"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="33"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34"/>
-      <c r="L37" s="35"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="30"/>
+      <c r="L37" s="31"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="33"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="34"/>
-      <c r="L38" s="35"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="31"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="33"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="34"/>
-      <c r="L39" s="35"/>
+      <c r="A39" s="29"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="31"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="33"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
-      <c r="K40" s="34"/>
-      <c r="L40" s="35"/>
+      <c r="A40" s="29"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="31"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="33"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="34"/>
-      <c r="K41" s="34"/>
-      <c r="L41" s="35"/>
+      <c r="A41" s="32"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="34"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="36"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="37"/>
-      <c r="L42" s="38"/>
+      <c r="A42" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="39"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="41"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="37"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
+      <c r="K44" s="30"/>
+      <c r="L44" s="31"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="33"/>
-      <c r="B45" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="42"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
-      <c r="K45" s="34"/>
-      <c r="L45" s="35"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="37"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
+      <c r="L45" s="31"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="33"/>
-      <c r="B46" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" s="42"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="35"/>
-    </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="45"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="46"/>
-      <c r="H47" s="46"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="46"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="47"/>
-    </row>
+      <c r="A46" s="40"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="42"/>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2610,7 +2570,7 @@
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="52">
@@ -2658,18 +2618,18 @@
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="B24:H24"/>
+    <mergeCell ref="A25:L25"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A27:L27"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="A42:L42"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:H44"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="D45:H45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:H46"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="54" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
address customer feedback for reports
</commit_message>
<xml_diff>
--- a/delivery_report_template.xlsx
+++ b/delivery_report_template.xlsx
@@ -20,15 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t xml:space="preserve">  Inspection Report  Substructure   Delivery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PV-Plant Name/Location:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Checking Company</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+  <si>
+    <t xml:space="preserve">Incoming Goods Inspection Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV Project:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subcontractor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S&amp;G Solar</t>
   </si>
   <si>
     <t xml:space="preserve">Delivery Details</t>
@@ -106,10 +112,25 @@
     <t xml:space="preserve">Inspected by and Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Printed Name:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date/Signature:</t>
+    <t xml:space="preserve">Name of installer:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signature:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of supervisor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of construction manager:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of inspector:</t>
   </si>
 </sst>
 </file>
@@ -122,7 +143,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -218,8 +239,41 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,11 +289,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -269,6 +329,20 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="medium"/>
       <top style="thin"/>
@@ -277,13 +351,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
@@ -299,13 +366,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
@@ -374,13 +434,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right/>
       <top/>
@@ -427,7 +480,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -449,42 +502,50 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -492,31 +553,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -524,11 +585,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -536,11 +597,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -568,15 +629,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -584,8 +669,36 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -593,10 +706,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -629,7 +738,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF8EAADB"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -670,6 +779,49 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>407160</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>105120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590760</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>39960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4836240" y="505080"/>
+          <a:ext cx="1955160" cy="735120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -852,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P30" activeCellId="0" sqref="P30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N55" activeCellId="0" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -891,7 +1043,9 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -901,14 +1055,16 @@
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="E3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
@@ -917,12 +1073,12 @@
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
@@ -931,12 +1087,12 @@
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6"/>
@@ -945,12 +1101,12 @@
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6"/>
@@ -959,645 +1115,826 @@
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="17"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="17"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="17"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="17"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="17"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="26"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="26"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="B20" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="26"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="15"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="B21" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="26"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="15"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="B22" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="26"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="15"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="B23" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="26"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="23" t="n">
         <v>7</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="15"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="15"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="15"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="15"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="L17" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="24"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="21" t="n">
+      <c r="B24" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="26"/>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="31"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="33"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="31"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="33"/>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="31"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="33"/>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="31"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="33"/>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="33"/>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="31"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="33"/>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="33"/>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="31"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="33"/>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="31"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="33"/>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="31"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="32"/>
+      <c r="L37" s="33"/>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="31"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="33"/>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="31"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="32"/>
+      <c r="L39" s="33"/>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="31"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
+      <c r="L40" s="33"/>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="36"/>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="30"/>
+      <c r="L42" s="30"/>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21" t="n">
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="9"/>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="31"/>
+      <c r="B44" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="39"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="G44" s="42"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J44" s="44"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="33"/>
+    </row>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="31"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="33"/>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="31"/>
+      <c r="B46" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="39"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" s="42"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="33"/>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="34"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="35"/>
+      <c r="L47" s="36"/>
+    </row>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="50"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="52"/>
+      <c r="L48" s="33"/>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="31"/>
+      <c r="B49" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="39"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" s="42"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J49" s="44"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="33"/>
+    </row>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="31"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="47"/>
+      <c r="K50" s="35"/>
+      <c r="L50" s="33"/>
+    </row>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="31"/>
+      <c r="B51" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="39"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="42"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J51" s="44"/>
+      <c r="K51" s="44"/>
+      <c r="L51" s="33"/>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="34"/>
+      <c r="B52" s="45"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="47"/>
+      <c r="K52" s="35"/>
+      <c r="L52" s="36"/>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="24"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21" t="n">
-        <v>4</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="24"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21" t="n">
-        <v>5</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="24"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21" t="n">
-        <v>6</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="21" t="n">
-        <v>7</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="29"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="31"/>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="31"/>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="31"/>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="29"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="31"/>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="29"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="31"/>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="29"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="31"/>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="31"/>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="29"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="31"/>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="29"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="31"/>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="29"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="31"/>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="29"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="31"/>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="29"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="31"/>
-    </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="29"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="31"/>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="32"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="34"/>
-    </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="35"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="5"/>
-    </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="29"/>
-      <c r="B44" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C44" s="37"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="31"/>
-    </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="29"/>
-      <c r="B45" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" s="37"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="31"/>
-    </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="40"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="41"/>
-      <c r="L46" s="42"/>
-    </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="51"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="51"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="53"/>
+      <c r="K53" s="52"/>
+      <c r="L53" s="33"/>
+    </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="31"/>
+      <c r="B54" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="39"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" s="42"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J54" s="44"/>
+      <c r="K54" s="44"/>
+      <c r="L54" s="33"/>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="31"/>
+      <c r="B55" s="45"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="47"/>
+      <c r="K55" s="35"/>
+      <c r="L55" s="33"/>
+    </row>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="31"/>
+      <c r="B56" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="39"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" s="42"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J56" s="44"/>
+      <c r="K56" s="44"/>
+      <c r="L56" s="33"/>
+    </row>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="54"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="55"/>
+      <c r="G57" s="55"/>
+      <c r="H57" s="55"/>
+      <c r="I57" s="55"/>
+      <c r="J57" s="55"/>
+      <c r="K57" s="55"/>
+      <c r="L57" s="56"/>
+    </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2527,16 +2864,28 @@
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="68">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I2:L7"/>
+    <mergeCell ref="I2:L2"/>
     <mergeCell ref="A3:D7"/>
-    <mergeCell ref="E3:H7"/>
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="F3:H7"/>
+    <mergeCell ref="I3:L7"/>
     <mergeCell ref="A8:L8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>
@@ -2580,9 +2929,23 @@
     <mergeCell ref="A27:L27"/>
     <mergeCell ref="A42:L42"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:H44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:H45"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="J56:K56"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2591,5 +2954,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix collage dimensions due to bug- WIP
</commit_message>
<xml_diff>
--- a/delivery_report_template.xlsx
+++ b/delivery_report_template.xlsx
@@ -143,7 +143,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -258,19 +258,7 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="5">
@@ -299,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -393,14 +381,28 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
-      <right/>
+      <right style="medium"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="medium"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -416,21 +418,14 @@
       <left/>
       <right style="medium"/>
       <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -606,74 +601,74 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -697,15 +692,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -792,9 +787,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>590760</xdr:colOff>
+      <xdr:colOff>590400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>39960</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -808,7 +803,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4836240" y="505080"/>
-          <a:ext cx="1955160" cy="735120"/>
+          <a:ext cx="1954800" cy="734760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1005,7 +1000,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N55" activeCellId="0" sqref="N55"/>
+      <selection pane="topLeft" activeCell="M39" activeCellId="0" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1473,199 +1468,199 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="33"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="31"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="33"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="31"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="33"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="31"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="33"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="31"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="33"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="31"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="33"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="31"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="33"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="31"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="33"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="31"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="33"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="31"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="33"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="31"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="33"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="31"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="33"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="31"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="33"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="34"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="35"/>
-      <c r="L41" s="36"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="30" t="s">
@@ -1684,88 +1679,88 @@
       <c r="L42" s="30"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
       <c r="L43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="31"/>
-      <c r="B44" s="39" t="s">
+      <c r="A44" s="34"/>
+      <c r="B44" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="39"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="41" t="s">
+      <c r="C44" s="35"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="G44" s="42"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="43" t="s">
+      <c r="G44" s="38"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="J44" s="44"/>
-      <c r="K44" s="44"/>
-      <c r="L44" s="33"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="41"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="31"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="35"/>
-      <c r="L45" s="33"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="41"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="31"/>
-      <c r="B46" s="39" t="s">
+      <c r="A46" s="34"/>
+      <c r="B46" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="39"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="40"/>
-      <c r="F46" s="41" t="s">
+      <c r="C46" s="35"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="G46" s="42"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="43" t="s">
+      <c r="G46" s="38"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="J46" s="44"/>
-      <c r="K46" s="44"/>
-      <c r="L46" s="33"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="41"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="34"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="46"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="35"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="35"/>
-      <c r="L47" s="36"/>
+      <c r="A47" s="46"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="45"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="47"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="48" t="s">
@@ -1781,75 +1776,75 @@
       <c r="I48" s="52"/>
       <c r="J48" s="53"/>
       <c r="K48" s="52"/>
-      <c r="L48" s="33"/>
+      <c r="L48" s="41"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="31"/>
-      <c r="B49" s="39" t="s">
+      <c r="A49" s="34"/>
+      <c r="B49" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="39"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="40"/>
-      <c r="F49" s="41" t="s">
+      <c r="C49" s="35"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="G49" s="42"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="43" t="s">
+      <c r="G49" s="38"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="J49" s="44"/>
-      <c r="K49" s="44"/>
-      <c r="L49" s="33"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="41"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="31"/>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="40"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="46"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="35"/>
-      <c r="J50" s="47"/>
-      <c r="K50" s="35"/>
-      <c r="L50" s="33"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="44"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="44"/>
+      <c r="L50" s="41"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="31"/>
-      <c r="B51" s="39" t="s">
+      <c r="A51" s="34"/>
+      <c r="B51" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="39"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="41" t="s">
+      <c r="C51" s="35"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="G51" s="42"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="43" t="s">
+      <c r="G51" s="38"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="J51" s="44"/>
-      <c r="K51" s="44"/>
-      <c r="L51" s="33"/>
+      <c r="J51" s="40"/>
+      <c r="K51" s="40"/>
+      <c r="L51" s="41"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="34"/>
-      <c r="B52" s="45"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="35"/>
-      <c r="J52" s="47"/>
-      <c r="K52" s="35"/>
-      <c r="L52" s="36"/>
+      <c r="A52" s="46"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="47"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="48" t="s">
@@ -1865,61 +1860,61 @@
       <c r="I53" s="52"/>
       <c r="J53" s="53"/>
       <c r="K53" s="52"/>
-      <c r="L53" s="33"/>
+      <c r="L53" s="41"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="31"/>
-      <c r="B54" s="39" t="s">
+      <c r="A54" s="34"/>
+      <c r="B54" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="39"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="41" t="s">
+      <c r="C54" s="35"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="G54" s="42"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="43" t="s">
+      <c r="G54" s="38"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="J54" s="44"/>
-      <c r="K54" s="44"/>
-      <c r="L54" s="33"/>
+      <c r="J54" s="40"/>
+      <c r="K54" s="40"/>
+      <c r="L54" s="41"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="31"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="46"/>
-      <c r="G55" s="46"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="35"/>
-      <c r="J55" s="47"/>
-      <c r="K55" s="35"/>
-      <c r="L55" s="33"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="44"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="44"/>
+      <c r="L55" s="41"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="31"/>
-      <c r="B56" s="39" t="s">
+      <c r="A56" s="34"/>
+      <c r="B56" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="39"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="41" t="s">
+      <c r="C56" s="35"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="G56" s="42"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="43" t="s">
+      <c r="G56" s="38"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="J56" s="44"/>
-      <c r="K56" s="44"/>
-      <c r="L56" s="33"/>
+      <c r="J56" s="40"/>
+      <c r="K56" s="40"/>
+      <c r="L56" s="41"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="54"/>
@@ -2877,7 +2872,7 @@
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="68">
+  <mergeCells count="69">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:H2"/>
@@ -2927,6 +2922,7 @@
     <mergeCell ref="A25:L25"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A27:L27"/>
+    <mergeCell ref="A28:L41"/>
     <mergeCell ref="A42:L42"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="D44:E44"/>

</xml_diff>

<commit_message>
remove hardcoded vars and extract them to base settings
</commit_message>
<xml_diff>
--- a/delivery_report_template.xlsx
+++ b/delivery_report_template.xlsx
@@ -324,13 +324,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="medium"/>
       <top style="thin"/>
@@ -354,6 +347,13 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
@@ -508,19 +508,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -532,15 +528,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -548,11 +544,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,7 +560,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -580,7 +576,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -592,11 +588,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -609,6 +605,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -780,16 +780,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>407160</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>833040</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>590400</xdr:colOff>
+      <xdr:colOff>129960</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:rowOff>142560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -802,8 +802,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4836240" y="505080"/>
-          <a:ext cx="1954800" cy="734760"/>
+          <a:off x="4376520" y="608760"/>
+          <a:ext cx="1954080" cy="734040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -999,8 +999,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M39" activeCellId="0" sqref="M39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1053,13 +1053,13 @@
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
@@ -1068,12 +1068,12 @@
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
@@ -1082,12 +1082,12 @@
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6"/>
@@ -1096,12 +1096,12 @@
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6"/>
@@ -1110,589 +1110,589 @@
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="17"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="17"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="17"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="17"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="17"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="17"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="16"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="21" t="s">
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="21" t="s">
+      <c r="J17" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="21" t="s">
+      <c r="K17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="22" t="s">
+      <c r="L17" s="21" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23" t="n">
+      <c r="A18" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="26"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="25"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="23" t="n">
+      <c r="A19" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="26"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="25"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="23" t="n">
+      <c r="A20" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="26"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="25"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="23" t="n">
+      <c r="A21" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="25"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="23" t="n">
+      <c r="A22" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="25"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="23" t="n">
+      <c r="A23" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="25"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="23" t="n">
+      <c r="A24" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="25"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="31"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="30"/>
+      <c r="L37" s="30"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="31"/>
-      <c r="L38" s="31"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
-      <c r="L39" s="31"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
+      <c r="L41" s="30"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="30"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="33"/>
-      <c r="L43" s="9"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="33"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="34"/>
@@ -2872,15 +2872,16 @@
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="69">
+  <mergeCells count="70">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="A3:D7"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="F3:H7"/>
-    <mergeCell ref="I3:L7"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="E4:H7"/>
+    <mergeCell ref="I4:L7"/>
     <mergeCell ref="A8:L8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>

</xml_diff>